<commit_message>
Merge two sorted arrays in place
</commit_message>
<xml_diff>
--- a/src/ProblemList.xlsx
+++ b/src/ProblemList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="16900" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="440" windowWidth="25040" windowHeight="17060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Arrays</t>
   </si>
@@ -40,6 +40,18 @@
   </si>
   <si>
     <t>FB, AMZN</t>
+  </si>
+  <si>
+    <t>Move Zeroes</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Find all palindromes of a string</t>
+  </si>
+  <si>
+    <t>AMZN</t>
   </si>
 </sst>
 </file>
@@ -474,7 +486,7 @@
   <dimension ref="A2:P42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -483,7 +495,9 @@
     <col min="2" max="2" width="19.5" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" style="3" customWidth="1"/>
     <col min="4" max="4" width="34.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="16" width="10.83203125" style="3"/>
+    <col min="5" max="5" width="10.83203125" style="3"/>
+    <col min="6" max="6" width="26.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:16" s="1" customFormat="1">
@@ -500,8 +514,12 @@
       <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -528,10 +546,22 @@
       <c r="E3" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="F3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="3">
         <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>

</xml_diff>